<commit_message>
cad and analysis updates
</commit_message>
<xml_diff>
--- a/Launches/8-inch-flight/Design/Calculations/trunk/Q-8in-motor_calc.xlsx
+++ b/Launches/8-inch-flight/Design/Calculations/trunk/Q-8in-motor_calc.xlsx
@@ -1628,6 +1628,132 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="15" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="2" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -1642,12 +1768,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -1691,173 +1811,17 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="41" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="40" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="2" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="46" xfId="2" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
@@ -1892,23 +1856,50 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="39" xfId="2" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="2" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="2" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="2" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="40" xfId="2" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="41" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="28" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="27" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="19" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="20" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="2" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
@@ -1922,17 +1913,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="23" xfId="2" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="6" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="37" xfId="6" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2462,94 +2462,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2612.3641311842121</c:v>
+                  <c:v>2663.2853736274451</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2720.2912381771334</c:v>
+                  <c:v>2771.0075317407118</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2826.4636514336025</c:v>
+                  <c:v>2876.9904164084619</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2930.3934462950788</c:v>
+                  <c:v>2980.7451726586405</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3031.5889676843672</c:v>
+                  <c:v>3081.7793177236772</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3129.5586250591318</c:v>
+                  <c:v>3179.6005242177857</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3223.8148041437935</c:v>
+                  <c:v>3273.7205218416875</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3313.8778538534334</c:v>
+                  <c:v>3363.6590757477015</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3399.2801044590219</c:v>
+                  <c:v>3448.9479973859661</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3479.5698713089373</c:v>
+                  <c:v>3529.1351419598327</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3554.3153973611934</c:v>
+                  <c:v>3603.7883455915062</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3623.1086874268481</c:v>
+                  <c:v>3672.4992549721942</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3685.5691873982187</c:v>
+                  <c:v>3734.8870026663849</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3741.3472628436607</c:v>
+                  <c:v>3790.6016823662194</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3790.1274331880491</c:v>
+                  <c:v>3839.3275802443941</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3831.6313202452206</c:v>
+                  <c:v>3880.7861211137511</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3865.6202730922046</c:v>
+                  <c:v>3914.738491335916</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3891.8976351290326</c:v>
+                  <c:v>3940.9879042843718</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3910.3106235928403</c:v>
+                  <c:v>3959.3814786001344</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3920.751796721097</c:v>
+                  <c:v>3969.8117044111568</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3923.1600891050684</c:v>
+                  <c:v>3972.2174780390969</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3917.5214014524076</c:v>
+                  <c:v>3966.5846914004251</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3903.8687368907258</c:v>
+                  <c:v>3952.9463682271512</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3882.2818819919044</c:v>
+                  <c:v>3931.3823452854199</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3852.886636775851</c:v>
+                  <c:v>3902.0185028542105</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3815.8536039584455</c:v>
+                  <c:v>3865.02555473757</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3771.3965535388102</c:v>
+                  <c:v>3820.6174139196191</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3719.7703843769095</c:v>
+                  <c:v>3769.0491555332374</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3661.2687096002337</c:v>
+                  <c:v>3710.6146040075237</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3596.2210974122804</c:v>
+                  <c:v>3645.6435760003365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4003,7 +4003,7 @@
   <dimension ref="A1:U996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4033,45 +4033,45 @@
   <sheetData>
     <row r="1" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="149" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="169"/>
-      <c r="D2" s="146" t="s">
+      <c r="C2" s="150"/>
+      <c r="D2" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="147"/>
+      <c r="E2" s="187"/>
       <c r="G2" s="86"/>
-      <c r="I2" s="135" t="s">
+      <c r="I2" s="177" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="136"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="136"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="136"/>
-      <c r="O2" s="136"/>
-      <c r="P2" s="137"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="178"/>
+      <c r="L2" s="178"/>
+      <c r="M2" s="178"/>
+      <c r="N2" s="178"/>
+      <c r="O2" s="178"/>
+      <c r="P2" s="179"/>
       <c r="Q2" s="3"/>
-      <c r="R2" s="184" t="s">
+      <c r="R2" s="168" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="184"/>
-      <c r="T2" s="172" t="b">
+      <c r="S2" s="168"/>
+      <c r="T2" s="155" t="b">
         <f>AND(ISNUMBER(D5),ISNUMBER(D6),ISNUMBER(D7),ISNUMBER(D8),ISNUMBER(D9),ISNUMBER(D10),ISNUMBER(D11),ISNUMBER(D12),NOT(ISBLANK($D$5:$D$12)))</f>
         <v>1</v>
       </c>
-      <c r="U2" s="172"/>
+      <c r="U2" s="155"/>
     </row>
     <row r="3" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="182" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144" t="s">
+      <c r="C3" s="183"/>
+      <c r="D3" s="184" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="145"/>
+      <c r="E3" s="185"/>
       <c r="G3" s="52"/>
       <c r="I3" s="51"/>
       <c r="J3" s="5"/>
@@ -4081,17 +4081,17 @@
       <c r="N3" s="52"/>
       <c r="O3" s="52"/>
       <c r="P3" s="7"/>
-      <c r="R3" s="185"/>
-      <c r="S3" s="185"/>
-      <c r="T3" s="173"/>
-      <c r="U3" s="173"/>
+      <c r="R3" s="169"/>
+      <c r="S3" s="169"/>
+      <c r="T3" s="156"/>
+      <c r="U3" s="156"/>
     </row>
     <row r="4" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G4" s="87"/>
-      <c r="I4" s="180" t="s">
+      <c r="I4" s="166" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="181"/>
+      <c r="J4" s="167"/>
       <c r="K4" s="37">
         <f>(($D$6-$D$7))/29</f>
         <v>0.14310344827586208</v>
@@ -4100,72 +4100,72 @@
         <v>58</v>
       </c>
       <c r="M4" s="52"/>
-      <c r="N4" s="154" t="s">
+      <c r="N4" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="155"/>
+      <c r="O4" s="136"/>
       <c r="P4" s="48">
         <f>Estimate!L4</f>
         <v>642.22020614588871</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="170" t="s">
+      <c r="B5" s="151" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="171"/>
+      <c r="C5" s="152"/>
       <c r="D5" s="42">
         <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="148" t="s">
+      <c r="F5" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="149"/>
-      <c r="I5" s="182" t="s">
+      <c r="G5" s="189"/>
+      <c r="I5" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="183"/>
+      <c r="J5" s="142"/>
       <c r="K5" s="38">
         <f>$M$16</f>
         <v>1103.146698363154</v>
       </c>
       <c r="L5" s="53"/>
       <c r="M5" s="52"/>
-      <c r="N5" s="166" t="s">
+      <c r="N5" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="167"/>
+      <c r="O5" s="148"/>
       <c r="P5" s="49">
         <f>Estimate!L5</f>
         <v>586.52275088831789</v>
       </c>
-      <c r="R5" s="174" t="s">
+      <c r="R5" s="157" t="s">
         <v>52</v>
       </c>
-      <c r="S5" s="175"/>
-      <c r="T5" s="175"/>
-      <c r="U5" s="176"/>
+      <c r="S5" s="158"/>
+      <c r="T5" s="158"/>
+      <c r="U5" s="159"/>
     </row>
     <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="153" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="139"/>
+      <c r="C6" s="154"/>
       <c r="D6" s="43">
         <v>6.9</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F6" s="150"/>
-      <c r="G6" s="151"/>
-      <c r="I6" s="182" t="s">
+      <c r="F6" s="190"/>
+      <c r="G6" s="191"/>
+      <c r="I6" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="183"/>
+      <c r="J6" s="142"/>
       <c r="K6" s="39">
         <f>PI()*Nozzle_Throat_Diameter^2/4</f>
         <v>4.0114996593688055</v>
@@ -4174,28 +4174,28 @@
         <v>42</v>
       </c>
       <c r="M6" s="52"/>
-      <c r="N6" s="166" t="s">
+      <c r="N6" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="167"/>
+      <c r="O6" s="148"/>
       <c r="P6" s="49">
         <f>Estimate!L6</f>
-        <v>3923.1600891050684</v>
+        <v>3972.2174780390969</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="177" t="str">
+      <c r="R6" s="160" t="str">
         <f>IF(ISNUMBER($D$5:$D$12), "", "Error: Input Values Must be Numerical")</f>
         <v/>
       </c>
-      <c r="S6" s="178"/>
-      <c r="T6" s="178"/>
-      <c r="U6" s="179"/>
+      <c r="S6" s="161"/>
+      <c r="T6" s="161"/>
+      <c r="U6" s="162"/>
     </row>
     <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="139"/>
+      <c r="C7" s="154"/>
       <c r="D7" s="64">
         <f>'Erosive Burning'!S5</f>
         <v>2.75</v>
@@ -4203,132 +4203,132 @@
       <c r="E7" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="152">
+      <c r="F7" s="192">
         <v>3</v>
       </c>
-      <c r="G7" s="153"/>
+      <c r="G7" s="193"/>
       <c r="H7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="182" t="s">
+      <c r="I7" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="183"/>
+      <c r="J7" s="142"/>
       <c r="K7" s="40">
         <f>$Q$16</f>
         <v>277.44592592592596</v>
       </c>
       <c r="L7" s="55"/>
       <c r="M7" s="52"/>
-      <c r="N7" s="166" t="s">
+      <c r="N7" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="O7" s="167"/>
+      <c r="O7" s="148"/>
       <c r="P7" s="49">
         <f>Estimate!L7</f>
-        <v>3550.8703801899906</v>
+        <v>3600.3926776300841</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="160" t="str">
+      <c r="R7" s="163" t="str">
         <f>IF(NOT(ISBLANK($D$5:$D$12)),"", "Error: Must Enter All Input Values")</f>
         <v/>
       </c>
-      <c r="S7" s="161"/>
-      <c r="T7" s="161"/>
-      <c r="U7" s="162"/>
+      <c r="S7" s="164"/>
+      <c r="T7" s="164"/>
+      <c r="U7" s="165"/>
     </row>
     <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="138" t="s">
+      <c r="B8" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="139"/>
+      <c r="C8" s="154"/>
       <c r="D8" s="43">
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="188">
+      <c r="F8" s="137">
         <v>3</v>
       </c>
-      <c r="G8" s="189"/>
+      <c r="G8" s="138"/>
       <c r="H8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="182" t="s">
+      <c r="I8" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="183"/>
+      <c r="J8" s="142"/>
       <c r="K8" s="40">
         <f>MAX(Q17:Q45)</f>
         <v>334.52647377460693</v>
       </c>
       <c r="L8" s="55"/>
       <c r="M8" s="52"/>
-      <c r="N8" s="166" t="s">
+      <c r="N8" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="O8" s="167"/>
+      <c r="O8" s="148"/>
       <c r="P8" s="49">
         <f>Estimate!L8</f>
         <v>9.2368014748779306</v>
       </c>
       <c r="Q8" s="3"/>
-      <c r="R8" s="160" t="str">
+      <c r="R8" s="163" t="str">
         <f>IF(ISNUMBER($F$7:$F$12), "", "Error: Grain Core Diameter Values Must be Numerical")</f>
         <v/>
       </c>
-      <c r="S8" s="161"/>
-      <c r="T8" s="161"/>
-      <c r="U8" s="162"/>
+      <c r="S8" s="164"/>
+      <c r="T8" s="164"/>
+      <c r="U8" s="165"/>
     </row>
     <row r="9" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="138" t="s">
+      <c r="B9" s="153" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="139"/>
+      <c r="C9" s="154"/>
       <c r="D9" s="43">
         <v>2.2599999999999998</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="188">
+      <c r="F9" s="137">
         <v>3</v>
       </c>
-      <c r="G9" s="189"/>
+      <c r="G9" s="138"/>
       <c r="H9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="192" t="s">
+      <c r="I9" s="143" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="193"/>
+      <c r="J9" s="144"/>
       <c r="K9" s="41">
         <f>$Q$45</f>
         <v>322.20444444444445</v>
       </c>
       <c r="L9" s="55"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="166" t="s">
+      <c r="N9" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="O9" s="167"/>
+      <c r="O9" s="148"/>
       <c r="P9" s="49">
         <f>Estimate!L9</f>
         <v>32626.648861105939</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="160"/>
-      <c r="S9" s="161"/>
-      <c r="T9" s="161"/>
-      <c r="U9" s="162"/>
+      <c r="R9" s="163"/>
+      <c r="S9" s="164"/>
+      <c r="T9" s="164"/>
+      <c r="U9" s="165"/>
     </row>
     <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="139"/>
+      <c r="C10" s="154"/>
       <c r="D10" s="64">
         <f>Nozzle_Throat_Diameter</f>
         <v>2.2599999999999998</v>
@@ -4336,10 +4336,10 @@
       <c r="E10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="190">
+      <c r="F10" s="139">
         <v>3.4</v>
       </c>
-      <c r="G10" s="191"/>
+      <c r="G10" s="140"/>
       <c r="H10" s="3" t="s">
         <v>54</v>
       </c>
@@ -4348,41 +4348,41 @@
       <c r="K10" s="56"/>
       <c r="L10" s="54"/>
       <c r="M10" s="52"/>
-      <c r="N10" s="156" t="s">
+      <c r="N10" s="173" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="157"/>
+      <c r="O10" s="174"/>
       <c r="P10" s="50">
         <f>MAX('Erosive Burning'!L14:L19)</f>
         <v>1.18406010621894</v>
       </c>
-      <c r="R10" s="163"/>
-      <c r="S10" s="164"/>
-      <c r="T10" s="164"/>
-      <c r="U10" s="165"/>
+      <c r="R10" s="170"/>
+      <c r="S10" s="171"/>
+      <c r="T10" s="171"/>
+      <c r="U10" s="172"/>
     </row>
     <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="138" t="s">
+      <c r="B11" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="139"/>
+      <c r="C11" s="154"/>
       <c r="D11" s="43">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="188">
+      <c r="F11" s="137">
         <v>3.8</v>
       </c>
-      <c r="G11" s="189"/>
+      <c r="G11" s="138"/>
       <c r="H11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="194" t="s">
+      <c r="I11" s="145" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="195"/>
+      <c r="J11" s="146"/>
       <c r="K11" s="44">
         <f>((D6*3)+D7)/2</f>
         <v>11.725000000000001</v>
@@ -4396,20 +4396,20 @@
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="180" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="141"/>
+      <c r="C12" s="181"/>
       <c r="D12" s="100">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="186">
+      <c r="F12" s="133">
         <v>4.3</v>
       </c>
-      <c r="G12" s="187"/>
+      <c r="G12" s="134"/>
       <c r="H12" s="2" t="s">
         <v>54</v>
       </c>
@@ -4417,20 +4417,20 @@
       <c r="J12" s="52"/>
       <c r="K12" s="52"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="154" t="s">
+      <c r="M12" s="135" t="s">
         <v>136</v>
       </c>
-      <c r="N12" s="155"/>
-      <c r="O12" s="158" t="s">
+      <c r="N12" s="136"/>
+      <c r="O12" s="194" t="s">
         <v>17</v>
       </c>
-      <c r="P12" s="159"/>
+      <c r="P12" s="195"/>
     </row>
     <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="133" t="s">
+      <c r="B13" s="175" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="134"/>
+      <c r="C13" s="176"/>
       <c r="D13" s="68">
         <f>(D10-D9)/29</f>
         <v>0</v>
@@ -4439,15 +4439,15 @@
       <c r="J13" s="58"/>
       <c r="K13" s="58"/>
       <c r="L13" s="58"/>
-      <c r="M13" s="156" t="s">
+      <c r="M13" s="173" t="s">
         <v>137</v>
       </c>
-      <c r="N13" s="157"/>
-      <c r="O13" s="233">
+      <c r="N13" s="174"/>
+      <c r="O13" s="196">
         <f>(36800+18400)/2</f>
         <v>27600</v>
       </c>
-      <c r="P13" s="234"/>
+      <c r="P13" s="197"/>
     </row>
     <row r="14" spans="1:21" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L14" s="4"/>
@@ -16185,37 +16185,6 @@
     <row r="996" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="T2:U3"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="R6:U6"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="R2:S3"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="R8:U8"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="I2:P2"/>
     <mergeCell ref="B9:C9"/>
@@ -16232,6 +16201,37 @@
     <mergeCell ref="O13:P13"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="R9:U9"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="T2:U3"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="R6:U6"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="R2:S3"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <conditionalFormatting sqref="T2:U3">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
@@ -16269,36 +16269,36 @@
   <sheetData>
     <row r="1" spans="2:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="218" t="s">
+      <c r="B2" s="206" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="220"/>
-      <c r="N2" s="212" t="s">
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="208"/>
+      <c r="N2" s="200" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="213"/>
-      <c r="P2" s="213"/>
-      <c r="Q2" s="213"/>
-      <c r="R2" s="213"/>
-      <c r="S2" s="213"/>
-      <c r="T2" s="214"/>
+      <c r="O2" s="201"/>
+      <c r="P2" s="201"/>
+      <c r="Q2" s="201"/>
+      <c r="R2" s="201"/>
+      <c r="S2" s="201"/>
+      <c r="T2" s="202"/>
     </row>
     <row r="3" spans="2:34" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="182" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="143"/>
-      <c r="D3" s="144" t="str">
+      <c r="C3" s="183"/>
+      <c r="D3" s="184" t="str">
         <f>'Bates Grain Kn Calculator'!D3</f>
         <v>Q-Motor</v>
       </c>
-      <c r="E3" s="145"/>
-      <c r="N3" s="201" t="s">
+      <c r="E3" s="185"/>
+      <c r="N3" s="218" t="s">
         <v>107</v>
       </c>
-      <c r="O3" s="203" t="s">
+      <c r="O3" s="220" t="s">
         <v>108</v>
       </c>
       <c r="P3" s="52"/>
@@ -16316,8 +16316,8 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="N4" s="201"/>
-      <c r="O4" s="203"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="220"/>
       <c r="P4" s="52"/>
       <c r="Q4" s="52"/>
       <c r="R4" s="52"/>
@@ -16325,11 +16325,11 @@
       <c r="T4" s="7"/>
     </row>
     <row r="5" spans="2:34" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="206" t="s">
+      <c r="B5" s="222" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="207"/>
-      <c r="D5" s="207"/>
+      <c r="C5" s="223"/>
+      <c r="D5" s="223"/>
       <c r="E5" s="66">
         <f>'Bates Grain Kn Calculator'!D6</f>
         <v>6.9</v>
@@ -16337,19 +16337,19 @@
       <c r="F5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="215" t="s">
+      <c r="H5" s="203" t="s">
         <v>126</v>
       </c>
-      <c r="I5" s="216"/>
-      <c r="J5" s="216"/>
-      <c r="K5" s="217"/>
-      <c r="N5" s="202"/>
-      <c r="O5" s="204"/>
+      <c r="I5" s="204"/>
+      <c r="J5" s="204"/>
+      <c r="K5" s="205"/>
+      <c r="N5" s="219"/>
+      <c r="O5" s="221"/>
       <c r="P5" s="52"/>
-      <c r="Q5" s="199" t="s">
+      <c r="Q5" s="209" t="s">
         <v>86</v>
       </c>
-      <c r="R5" s="200"/>
+      <c r="R5" s="217"/>
       <c r="S5" s="132">
         <v>2.75</v>
       </c>
@@ -16358,11 +16358,11 @@
       </c>
     </row>
     <row r="6" spans="2:34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="208" t="s">
+      <c r="B6" s="213" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="209"/>
-      <c r="D6" s="209"/>
+      <c r="C6" s="214"/>
+      <c r="D6" s="214"/>
       <c r="E6" s="67">
         <f>'Bates Grain Kn Calculator'!D8</f>
         <v>14</v>
@@ -16370,11 +16370,11 @@
       <c r="F6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="199" t="s">
+      <c r="H6" s="209" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="221"/>
-      <c r="J6" s="221"/>
+      <c r="I6" s="210"/>
+      <c r="J6" s="210"/>
       <c r="K6" s="65">
         <v>0.57499999999999996</v>
       </c>
@@ -16390,10 +16390,10 @@
         <v>424.53912324285676</v>
       </c>
       <c r="P6" s="52"/>
-      <c r="Q6" s="197" t="s">
+      <c r="Q6" s="211" t="s">
         <v>89</v>
       </c>
-      <c r="R6" s="198"/>
+      <c r="R6" s="216"/>
       <c r="S6" s="76">
         <f>AVERAGE(E14:E19)</f>
         <v>28.034787442471924</v>
@@ -16403,22 +16403,22 @@
       </c>
     </row>
     <row r="7" spans="2:34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="208" t="s">
+      <c r="B7" s="213" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="209"/>
-      <c r="D7" s="209"/>
+      <c r="C7" s="214"/>
+      <c r="D7" s="214"/>
       <c r="E7" s="62">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="197" t="s">
+      <c r="H7" s="211" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="205"/>
-      <c r="J7" s="205"/>
+      <c r="I7" s="212"/>
+      <c r="J7" s="212"/>
       <c r="K7" s="65">
         <v>0.1</v>
       </c>
@@ -16434,10 +16434,10 @@
         <v>424.53912324285676</v>
       </c>
       <c r="P7" s="52"/>
-      <c r="Q7" s="197" t="s">
+      <c r="Q7" s="211" t="s">
         <v>88</v>
       </c>
-      <c r="R7" s="198"/>
+      <c r="R7" s="216"/>
       <c r="S7" s="76">
         <f>(C14+C15+C16+C17+C18+C19)/ng</f>
         <v>3.4166666666666665</v>
@@ -16447,11 +16447,11 @@
       </c>
     </row>
     <row r="8" spans="2:34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="208" t="s">
+      <c r="B8" s="213" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="209"/>
-      <c r="D8" s="209"/>
+      <c r="C8" s="214"/>
+      <c r="D8" s="214"/>
       <c r="E8" s="67">
         <f>Estimate!D10</f>
         <v>0.23289725920790463</v>
@@ -16459,11 +16459,11 @@
       <c r="F8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="197" t="s">
+      <c r="H8" s="211" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="205"/>
-      <c r="J8" s="205"/>
+      <c r="I8" s="212"/>
+      <c r="J8" s="212"/>
       <c r="K8" s="65">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -16479,10 +16479,10 @@
         <v>424.53912324285676</v>
       </c>
       <c r="P8" s="52"/>
-      <c r="Q8" s="197" t="s">
+      <c r="Q8" s="211" t="s">
         <v>87</v>
       </c>
-      <c r="R8" s="198"/>
+      <c r="R8" s="216"/>
       <c r="S8" s="76">
         <f>SUM(O6:O11)</f>
         <v>2354.9221451676417</v>
@@ -16492,11 +16492,11 @@
       </c>
     </row>
     <row r="9" spans="2:34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="208" t="s">
+      <c r="B9" s="213" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="209"/>
-      <c r="D9" s="209"/>
+      <c r="C9" s="214"/>
+      <c r="D9" s="214"/>
       <c r="E9" s="67">
         <f>[0]!Num_Grains</f>
         <v>6</v>
@@ -16504,11 +16504,11 @@
       <c r="F9" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="197" t="s">
+      <c r="H9" s="211" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="205"/>
-      <c r="J9" s="205"/>
+      <c r="I9" s="212"/>
+      <c r="J9" s="212"/>
       <c r="K9" s="65">
         <f>PI()/4*ds^2</f>
         <v>0.25967226777328128</v>
@@ -16525,10 +16525,10 @@
         <v>396.39045306669226</v>
       </c>
       <c r="P9" s="52"/>
-      <c r="Q9" s="197" t="s">
+      <c r="Q9" s="211" t="s">
         <v>84</v>
       </c>
-      <c r="R9" s="198"/>
+      <c r="R9" s="216"/>
       <c r="S9" s="76">
         <f>S10*rhop</f>
         <v>138.94040656489085</v>
@@ -16538,11 +16538,11 @@
       </c>
     </row>
     <row r="10" spans="2:34" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="210" t="s">
+      <c r="B10" s="198" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="211"/>
-      <c r="D10" s="211"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="199"/>
       <c r="E10" s="75">
         <f>[0]!boundary_layer</f>
         <v>5.0000000000000001E-3</v>
@@ -16550,11 +16550,11 @@
       <c r="F10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H10" s="197" t="s">
+      <c r="H10" s="211" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="205"/>
-      <c r="J10" s="205"/>
+      <c r="I10" s="212"/>
+      <c r="J10" s="212"/>
       <c r="K10" s="65">
         <f>As*sdots</f>
         <v>2.5967226777328128E-2</v>
@@ -16571,10 +16571,10 @@
         <v>364.72319911850713</v>
       </c>
       <c r="P10" s="52"/>
-      <c r="Q10" s="133" t="s">
+      <c r="Q10" s="175" t="s">
         <v>85</v>
       </c>
-      <c r="R10" s="134"/>
+      <c r="R10" s="176"/>
       <c r="S10" s="77">
         <f>S8</f>
         <v>2354.9221451676417</v>
@@ -16591,11 +16591,11 @@
       <c r="AH10" s="3"/>
     </row>
     <row r="11" spans="2:34" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="175" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="196"/>
-      <c r="D11" s="134"/>
+      <c r="C11" s="215"/>
+      <c r="D11" s="176"/>
       <c r="E11" s="63">
         <v>1.4</v>
       </c>
@@ -16603,11 +16603,11 @@
         <v>92</v>
       </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="133" t="s">
+      <c r="H11" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="196"/>
-      <c r="J11" s="196"/>
+      <c r="I11" s="215"/>
+      <c r="J11" s="215"/>
       <c r="K11" s="68">
         <f>Vdots*rhos</f>
         <v>1.8177058744129691E-3</v>
@@ -21237,16 +21237,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="N2:T2"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="Q9:R9"/>
     <mergeCell ref="Q10:R10"/>
@@ -21263,6 +21253,16 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -21289,14 +21289,14 @@
   <sheetData>
     <row r="1" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="231" t="s">
+      <c r="B2" s="230" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="232"/>
-      <c r="F2" s="227" t="s">
+      <c r="C2" s="231"/>
+      <c r="F2" s="224" t="s">
         <v>133</v>
       </c>
-      <c r="G2" s="228"/>
+      <c r="G2" s="225"/>
       <c r="H2" s="120">
         <v>1.26</v>
       </c>
@@ -21310,22 +21310,22 @@
       <c r="O3" s="3"/>
     </row>
     <row r="4" spans="2:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="209" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="200"/>
+      <c r="C4" s="217"/>
       <c r="D4" s="83">
         <v>9.1</v>
       </c>
-      <c r="F4" s="224" t="s">
+      <c r="F4" s="232" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="225"/>
-      <c r="H4" s="226"/>
-      <c r="J4" s="206" t="s">
+      <c r="G4" s="233"/>
+      <c r="H4" s="234"/>
+      <c r="J4" s="222" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="207"/>
+      <c r="K4" s="223"/>
       <c r="L4" s="121">
         <f>MAX(D14:D43)</f>
         <v>642.22020614588871</v>
@@ -21335,24 +21335,24 @@
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="2:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="211" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="198"/>
+      <c r="C5" s="216"/>
       <c r="D5" s="84">
         <v>13.43</v>
       </c>
-      <c r="F5" s="208" t="s">
+      <c r="F5" s="213" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="209"/>
+      <c r="G5" s="214"/>
       <c r="H5" s="117">
         <v>1.4109999999999999E-2</v>
       </c>
-      <c r="J5" s="208" t="s">
+      <c r="J5" s="213" t="s">
         <v>128</v>
       </c>
-      <c r="K5" s="209"/>
+      <c r="K5" s="214"/>
       <c r="L5" s="128">
         <f>AVERAGE(D14:D43)</f>
         <v>586.52275088831789</v>
@@ -21362,28 +21362,28 @@
       <c r="O5" s="3"/>
     </row>
     <row r="6" spans="2:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="197" t="s">
+      <c r="B6" s="211" t="s">
         <v>119</v>
       </c>
-      <c r="C6" s="198"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="84">
         <f>(('Bates Grain Kn Calculator'!D11^2)/4)/((Nozzle_Throat_Diameter^2)/4)</f>
-        <v>15.858720338319371</v>
-      </c>
-      <c r="F6" s="208" t="s">
+        <v>7.048320150364165</v>
+      </c>
+      <c r="F6" s="213" t="s">
         <v>132</v>
       </c>
-      <c r="G6" s="209"/>
+      <c r="G6" s="214"/>
       <c r="H6" s="117">
         <v>0.44005699999999998</v>
       </c>
-      <c r="J6" s="208" t="s">
+      <c r="J6" s="213" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="209"/>
+      <c r="K6" s="214"/>
       <c r="L6" s="122">
         <f>MAX(L14:L43)</f>
-        <v>3923.1600891050684</v>
+        <v>3972.2174780390969</v>
       </c>
       <c r="M6" s="81" t="s">
         <v>56</v>
@@ -21391,46 +21391,46 @@
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="2:29" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="197" t="s">
+      <c r="B7" s="211" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="198"/>
+      <c r="C7" s="216"/>
       <c r="D7" s="84">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F7" s="229"/>
-      <c r="G7" s="230"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="227"/>
       <c r="H7" s="101"/>
-      <c r="J7" s="208" t="s">
+      <c r="J7" s="213" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="209"/>
+      <c r="K7" s="214"/>
       <c r="L7" s="122">
         <f>AVERAGE(L14:L43)</f>
-        <v>3550.8703801899906</v>
+        <v>3600.3926776300841</v>
       </c>
       <c r="M7" s="81" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="211" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="198"/>
+      <c r="C8" s="216"/>
       <c r="D8" s="84">
         <f>6*2300</f>
         <v>13800</v>
       </c>
-      <c r="F8" s="224" t="s">
+      <c r="F8" s="232" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="225"/>
-      <c r="H8" s="226"/>
-      <c r="J8" s="208" t="s">
+      <c r="G8" s="233"/>
+      <c r="H8" s="234"/>
+      <c r="J8" s="213" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="209"/>
+      <c r="K8" s="214"/>
       <c r="L8" s="123">
         <f>K43</f>
         <v>9.2368014748779306</v>
@@ -21441,26 +21441,26 @@
       <c r="V8" s="3"/>
     </row>
     <row r="9" spans="2:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="211" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="198"/>
+      <c r="C9" s="216"/>
       <c r="D9" s="84">
         <f>AVERAGE(D14:D43)</f>
         <v>586.52275088831789</v>
       </c>
-      <c r="F9" s="208" t="s">
+      <c r="F9" s="213" t="s">
         <v>129</v>
       </c>
-      <c r="G9" s="209"/>
+      <c r="G9" s="214"/>
       <c r="H9" s="118">
         <v>75.234999999999999</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="208" t="s">
+      <c r="J9" s="213" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="209"/>
+      <c r="K9" s="214"/>
       <c r="L9" s="122">
         <f>MAX(M14:M43)</f>
         <v>32626.648861105939</v>
@@ -21470,26 +21470,26 @@
       </c>
     </row>
     <row r="10" spans="2:29" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="175" t="s">
         <v>123</v>
       </c>
-      <c r="C10" s="134"/>
+      <c r="C10" s="176"/>
       <c r="D10" s="85">
         <f>AVERAGE(I14:I43)</f>
         <v>0.23289725920790463</v>
       </c>
-      <c r="F10" s="222" t="s">
+      <c r="F10" s="228" t="s">
         <v>130</v>
       </c>
-      <c r="G10" s="223"/>
+      <c r="G10" s="229"/>
       <c r="H10" s="119">
         <v>6.4099999999999999E-3</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="222" t="s">
+      <c r="J10" s="228" t="s">
         <v>127</v>
       </c>
-      <c r="K10" s="223"/>
+      <c r="K10" s="229"/>
       <c r="L10" s="124">
         <f>L9/'Erosive Burning'!S9</f>
         <v>234.82476889016414</v>
@@ -21584,11 +21584,11 @@
       </c>
       <c r="F14" s="89">
         <f t="shared" ref="F14:F43" si="0">SQRT((((2*$H$2^2)/($H$2-1))*((2/($H$2+1))^(($H$2+1)/($H$2-1))*(1-(($D$4/D14)^(($H$2-1)/$H$2)))))+($D$6*(($D$4-$D$5)/D14)))</f>
-        <v>1.4750177109747984</v>
+        <v>1.5037693438624242</v>
       </c>
       <c r="G14" s="89">
         <f t="shared" ref="G14:G43" si="1">(D14*E14)*F14</f>
-        <v>2612.3641311842121</v>
+        <v>2663.2853736274451</v>
       </c>
       <c r="H14" s="104">
         <f>'Bates Grain Kn Calculator'!N16-'Bates Grain Kn Calculator'!N17</f>
@@ -21607,7 +21607,7 @@
       </c>
       <c r="L14" s="89">
         <f t="shared" ref="L14:L43" si="4">G14</f>
-        <v>2612.3641311842121</v>
+        <v>2663.2853736274451</v>
       </c>
       <c r="M14" s="105">
         <v>904.71529973261499</v>
@@ -21628,7 +21628,7 @@
         <v>283.06683930065617</v>
       </c>
       <c r="D15" s="115">
-        <f t="shared" ref="D14:D43" si="5">($H$9*EXP(C15*$H$10))</f>
+        <f t="shared" ref="D15:D43" si="5">($H$9*EXP(C15*$H$10))</f>
         <v>461.77372026747497</v>
       </c>
       <c r="E15" s="107">
@@ -21637,11 +21637,11 @@
       </c>
       <c r="F15" s="93">
         <f t="shared" si="0"/>
-        <v>1.4816010315160608</v>
+        <v>1.5092235565618797</v>
       </c>
       <c r="G15" s="93">
         <f t="shared" si="1"/>
-        <v>2720.2912381771334</v>
+        <v>2771.0075317407118</v>
       </c>
       <c r="H15" s="108">
         <f>'Bates Grain Kn Calculator'!N17-'Bates Grain Kn Calculator'!N18</f>
@@ -21660,7 +21660,7 @@
       </c>
       <c r="L15" s="93">
         <f t="shared" si="4"/>
-        <v>2720.2912381771334</v>
+        <v>2771.0075317407118</v>
       </c>
       <c r="M15" s="109">
         <v>1831.9886229695926</v>
@@ -21690,11 +21690,11 @@
       </c>
       <c r="F16" s="93">
         <f t="shared" si="0"/>
-        <v>1.4877241497602827</v>
+        <v>1.5143191807716432</v>
       </c>
       <c r="G16" s="93">
         <f t="shared" si="1"/>
-        <v>2826.4636514336025</v>
+        <v>2876.9904164084619</v>
       </c>
       <c r="H16" s="108">
         <f>'Bates Grain Kn Calculator'!N18-'Bates Grain Kn Calculator'!N19</f>
@@ -21713,7 +21713,7 @@
       </c>
       <c r="L16" s="93">
         <f t="shared" si="4"/>
-        <v>2826.4636514336025</v>
+        <v>2876.9904164084619</v>
       </c>
       <c r="M16" s="109">
         <v>2781.0771058229193</v>
@@ -21743,11 +21743,11 @@
       </c>
       <c r="F17" s="93">
         <f t="shared" si="0"/>
-        <v>1.493409379126277</v>
+        <v>1.5190700085894002</v>
       </c>
       <c r="G17" s="93">
         <f t="shared" si="1"/>
-        <v>2930.3934462950788</v>
+        <v>2980.7451726586405</v>
       </c>
       <c r="H17" s="108">
         <f>'Bates Grain Kn Calculator'!N19-'Bates Grain Kn Calculator'!N20</f>
@@ -21766,7 +21766,7 @@
       </c>
       <c r="L17" s="93">
         <f t="shared" si="4"/>
-        <v>2930.3934462950788</v>
+        <v>2980.7451726586405</v>
       </c>
       <c r="M17" s="109">
         <v>3751.1781309650551</v>
@@ -21796,11 +21796,11 @@
       </c>
       <c r="F18" s="93">
         <f t="shared" si="0"/>
-        <v>1.4986767960031118</v>
+        <v>1.5234885741791759</v>
       </c>
       <c r="G18" s="93">
         <f t="shared" si="1"/>
-        <v>3031.5889676843672</v>
+        <v>3081.7793177236772</v>
       </c>
       <c r="H18" s="108">
         <f>'Bates Grain Kn Calculator'!N20-'Bates Grain Kn Calculator'!N21</f>
@@ -21819,7 +21819,7 @@
       </c>
       <c r="L18" s="93">
         <f t="shared" si="4"/>
-        <v>3031.5889676843672</v>
+        <v>3081.7793177236772</v>
       </c>
       <c r="M18" s="109">
         <v>4741.4304607778377</v>
@@ -21849,11 +21849,11 @@
       </c>
       <c r="F19" s="93">
         <f t="shared" si="0"/>
-        <v>1.5035444601589307</v>
+        <v>1.5275862594252423</v>
       </c>
       <c r="G19" s="93">
         <f t="shared" si="1"/>
-        <v>3129.5586250591318</v>
+        <v>3179.6005242177857</v>
       </c>
       <c r="H19" s="108">
         <f>'Bates Grain Kn Calculator'!N21-'Bates Grain Kn Calculator'!N22</f>
@@ -21872,7 +21872,7 @@
       </c>
       <c r="L19" s="93">
         <f t="shared" si="4"/>
-        <v>3129.5586250591318</v>
+        <v>3179.6005242177857</v>
       </c>
       <c r="M19" s="109">
         <v>5750.9156866625472</v>
@@ -21902,11 +21902,11 @@
       </c>
       <c r="F20" s="93">
         <f t="shared" si="0"/>
-        <v>1.5080286058392234</v>
+        <v>1.531373386620869</v>
       </c>
       <c r="G20" s="93">
         <f t="shared" si="1"/>
-        <v>3223.8148041437935</v>
+        <v>3273.7205218416875</v>
       </c>
       <c r="H20" s="108">
         <f>'Bates Grain Kn Calculator'!N22-'Bates Grain Kn Calculator'!N23</f>
@@ -21925,7 +21925,7 @@
       </c>
       <c r="L20" s="93">
         <f t="shared" si="4"/>
-        <v>3223.8148041437935</v>
+        <v>3273.7205218416875</v>
       </c>
       <c r="M20" s="109">
         <v>6778.6599875226448</v>
@@ -21955,11 +21955,11 @@
       </c>
       <c r="F21" s="93">
         <f t="shared" si="0"/>
-        <v>1.5121438076589107</v>
+        <v>1.5348592998239521</v>
       </c>
       <c r="G21" s="93">
         <f t="shared" si="1"/>
-        <v>3313.8778538534334</v>
+        <v>3363.6590757477015</v>
       </c>
       <c r="H21" s="108">
         <f>'Bates Grain Kn Calculator'!N23-'Bates Grain Kn Calculator'!N24</f>
@@ -21978,7 +21978,7 @@
       </c>
       <c r="L21" s="93">
         <f t="shared" si="4"/>
-        <v>3313.8778538534334</v>
+        <v>3363.6590757477015</v>
       </c>
       <c r="M21" s="109">
         <v>7823.6361889164873</v>
@@ -22008,11 +22008,11 @@
       </c>
       <c r="F22" s="93">
         <f t="shared" si="0"/>
-        <v>1.5159031247113479</v>
+        <v>1.5380524362632317</v>
       </c>
       <c r="G22" s="93">
         <f t="shared" si="1"/>
-        <v>3399.2801044590219</v>
+        <v>3448.9479973859661</v>
       </c>
       <c r="H22" s="108">
         <f>'Bates Grain Kn Calculator'!N24-'Bates Grain Kn Calculator'!N25</f>
@@ -22031,7 +22031,7 @@
       </c>
       <c r="L22" s="93">
         <f t="shared" si="4"/>
-        <v>3399.2801044590219</v>
+        <v>3448.9479973859661</v>
       </c>
       <c r="M22" s="109">
         <v>8884.766112800984</v>
@@ -22061,11 +22061,11 @@
       </c>
       <c r="F23" s="93">
         <f t="shared" si="0"/>
-        <v>1.5193182257576041</v>
+        <v>1.5409603889702042</v>
       </c>
       <c r="G23" s="93">
         <f t="shared" si="1"/>
-        <v>3479.5698713089373</v>
+        <v>3529.1351419598327</v>
       </c>
       <c r="H23" s="108">
         <f>'Bates Grain Kn Calculator'!N25-'Bates Grain Kn Calculator'!N26</f>
@@ -22084,7 +22084,7 @@
       </c>
       <c r="L23" s="93">
         <f t="shared" si="4"/>
-        <v>3479.5698713089373</v>
+        <v>3529.1351419598327</v>
       </c>
       <c r="M23" s="109">
         <v>9960.9232061793537</v>
@@ -22114,11 +22114,11 @@
       </c>
       <c r="F24" s="93">
         <f t="shared" si="0"/>
-        <v>1.5223994978966091</v>
+        <v>1.5435899616357613</v>
       </c>
       <c r="G24" s="93">
         <f t="shared" si="1"/>
-        <v>3554.3153973611934</v>
+        <v>3603.7883455915062</v>
       </c>
       <c r="H24" s="108">
         <f>'Bates Grain Kn Calculator'!N26-'Bates Grain Kn Calculator'!N27</f>
@@ -22137,7 +22137,7 @@
       </c>
       <c r="L24" s="93">
         <f t="shared" si="4"/>
-        <v>3554.3153973611934</v>
+        <v>3603.7883455915062</v>
       </c>
       <c r="M24" s="109">
         <v>11050.935435354861</v>
@@ -22167,11 +22167,11 @@
       </c>
       <c r="F25" s="93">
         <f t="shared" si="0"/>
-        <v>1.5251561407317806</v>
+        <v>1.5459472165411876</v>
       </c>
       <c r="G25" s="93">
         <f t="shared" si="1"/>
-        <v>3623.1086874268481</v>
+        <v>3672.4992549721942</v>
       </c>
       <c r="H25" s="108">
         <f>'Bates Grain Kn Calculator'!N27-'Bates Grain Kn Calculator'!N28</f>
@@ -22190,7 +22190,7 @@
       </c>
       <c r="L25" s="93">
         <f t="shared" si="4"/>
-        <v>3623.1086874268481</v>
+        <v>3672.4992549721942</v>
       </c>
       <c r="M25" s="109">
         <v>12153.588430903163</v>
@@ -22220,11 +22220,11 @@
       </c>
       <c r="F26" s="93">
         <f t="shared" si="0"/>
-        <v>1.5275962477273854</v>
+        <v>1.5480375162856748</v>
       </c>
       <c r="G26" s="93">
         <f t="shared" si="1"/>
-        <v>3685.5691873982187</v>
+        <v>3734.8870026663849</v>
       </c>
       <c r="H26" s="108">
         <f>'Bates Grain Kn Calculator'!N28-'Bates Grain Kn Calculator'!N29</f>
@@ -22243,7 +22243,7 @@
       </c>
       <c r="L26" s="93">
         <f t="shared" si="4"/>
-        <v>3685.5691873982187</v>
+        <v>3734.8870026663849</v>
       </c>
       <c r="M26" s="109">
         <v>13267.628866931094</v>
@@ -22273,11 +22273,11 @@
       </c>
       <c r="F27" s="93">
         <f t="shared" si="0"/>
-        <v>1.5297268761761222</v>
+        <v>1.5498655599231219</v>
       </c>
       <c r="G27" s="93">
         <f t="shared" si="1"/>
-        <v>3741.3472628436607</v>
+        <v>3790.6016823662194</v>
       </c>
       <c r="H27" s="108">
         <f>'Bates Grain Kn Calculator'!N29-'Bates Grain Kn Calculator'!N30</f>
@@ -22296,7 +22296,7 @@
       </c>
       <c r="L27" s="93">
         <f t="shared" si="4"/>
-        <v>3741.3472628436607</v>
+        <v>3790.6016823662194</v>
       </c>
       <c r="M27" s="109">
         <v>14391.768056711462</v>
@@ -22326,11 +22326,11 @@
       </c>
       <c r="F28" s="93">
         <f t="shared" si="0"/>
-        <v>1.5315541069686216</v>
+        <v>1.551435414026475</v>
       </c>
       <c r="G28" s="93">
         <f t="shared" si="1"/>
-        <v>3790.1274331880491</v>
+        <v>3839.3275802443941</v>
       </c>
       <c r="H28" s="108">
         <f>'Bates Grain Kn Calculator'!N30-'Bates Grain Kn Calculator'!N31</f>
@@ -22349,7 +22349,7 @@
       </c>
       <c r="L28" s="93">
         <f t="shared" si="4"/>
-        <v>3790.1274331880491</v>
+        <v>3839.3275802443941</v>
       </c>
       <c r="M28" s="109">
         <v>15524.68574539031</v>
@@ -22379,11 +22379,11 @@
       </c>
       <c r="F29" s="93">
         <f t="shared" si="0"/>
-        <v>1.5330830951579257</v>
+        <v>1.5527505391156016</v>
       </c>
       <c r="G29" s="93">
         <f t="shared" si="1"/>
-        <v>3831.6313202452206</v>
+        <v>3880.7861211137511</v>
       </c>
       <c r="H29" s="108">
         <f>'Bates Grain Kn Calculator'!N31-'Bates Grain Kn Calculator'!N32</f>
@@ -22402,7 +22402,7 @@
       </c>
       <c r="L29" s="93">
         <f t="shared" si="4"/>
-        <v>3831.6313202452206</v>
+        <v>3880.7861211137511</v>
       </c>
       <c r="M29" s="109">
         <v>16665.03407917271</v>
@@ -22432,11 +22432,11 @@
       </c>
       <c r="F30" s="93">
         <f t="shared" si="0"/>
-        <v>1.5343181121412168</v>
+        <v>1.5538138118125007</v>
       </c>
       <c r="G30" s="93">
         <f t="shared" si="1"/>
-        <v>3865.6202730922046</v>
+        <v>3914.738491335916</v>
       </c>
       <c r="H30" s="108">
         <f>'Bates Grain Kn Calculator'!N32-'Bates Grain Kn Calculator'!N33</f>
@@ -22455,7 +22455,7 @@
       </c>
       <c r="L30" s="93">
         <f t="shared" si="4"/>
-        <v>3865.6202730922046</v>
+        <v>3914.738491335916</v>
       </c>
       <c r="M30" s="109">
         <v>17811.441729221737</v>
@@ -22485,11 +22485,11 @@
       </c>
       <c r="F31" s="93">
         <f t="shared" si="0"/>
-        <v>1.5352625801318753</v>
+        <v>1.5546275430236334</v>
       </c>
       <c r="G31" s="93">
         <f t="shared" si="1"/>
-        <v>3891.8976351290326</v>
+        <v>3940.9879042843718</v>
       </c>
       <c r="H31" s="108">
         <f>'Bates Grain Kn Calculator'!N33-'Bates Grain Kn Calculator'!N34</f>
@@ -22508,7 +22508,7 @@
       </c>
       <c r="L31" s="93">
         <f t="shared" si="4"/>
-        <v>3891.8976351290326</v>
+        <v>3940.9879042843718</v>
       </c>
       <c r="M31" s="109">
         <v>18962.51814746625</v>
@@ -22538,11 +22538,11 @@
       </c>
       <c r="F32" s="93">
         <f t="shared" si="0"/>
-        <v>1.5359190994630392</v>
+        <v>1.5551934923918123</v>
       </c>
       <c r="G32" s="93">
         <f t="shared" si="1"/>
-        <v>3910.3106235928403</v>
+        <v>3959.3814786001344</v>
       </c>
       <c r="H32" s="108">
         <f>'Bates Grain Kn Calculator'!N34-'Bates Grain Kn Calculator'!N35</f>
@@ -22561,7 +22561,7 @@
       </c>
       <c r="L32" s="93">
         <f t="shared" si="4"/>
-        <v>3910.3106235928403</v>
+        <v>3959.3814786001344</v>
       </c>
       <c r="M32" s="109">
         <v>20116.857930618917</v>
@@ -22591,11 +22591,11 @@
       </c>
       <c r="F33" s="93">
         <f t="shared" si="0"/>
-        <v>1.5362894691454851</v>
+        <v>1.5555128792079431</v>
       </c>
       <c r="G33" s="93">
         <f t="shared" si="1"/>
-        <v>3920.751796721097</v>
+        <v>3969.8117044111568</v>
       </c>
       <c r="H33" s="108">
         <f>'Bates Grain Kn Calculator'!N35-'Bates Grain Kn Calculator'!N36</f>
@@ -22614,7 +22614,7 @@
       </c>
       <c r="L33" s="93">
         <f t="shared" si="4"/>
-        <v>3920.751796721097</v>
+        <v>3969.8117044111568</v>
       </c>
       <c r="M33" s="109">
         <v>21273.04526796686</v>
@@ -22644,11 +22644,11 @@
       </c>
       <c r="F34" s="93">
         <f t="shared" si="0"/>
-        <v>1.536374700994759</v>
+        <v>1.555586389924918</v>
       </c>
       <c r="G34" s="93">
         <f t="shared" si="1"/>
-        <v>3923.1600891050684</v>
+        <v>3972.2174780390969</v>
       </c>
       <c r="H34" s="108">
         <f>'Bates Grain Kn Calculator'!N36-'Bates Grain Kn Calculator'!N37</f>
@@ -22667,7 +22667,7 @@
       </c>
       <c r="L34" s="93">
         <f t="shared" si="4"/>
-        <v>3923.1600891050684</v>
+        <v>3972.2174780390969</v>
       </c>
       <c r="M34" s="109">
         <v>22429.658447921935</v>
@@ -22697,11 +22697,11 @@
       </c>
       <c r="F35" s="93">
         <f t="shared" si="0"/>
-        <v>1.5361750275422363</v>
+        <v>1.5554141823709158</v>
       </c>
       <c r="G35" s="93">
         <f t="shared" si="1"/>
-        <v>3917.5214014524076</v>
+        <v>3966.5846914004251</v>
       </c>
       <c r="H35" s="108">
         <f>'Bates Grain Kn Calculator'!N37-'Bates Grain Kn Calculator'!N38</f>
@@ -22720,7 +22720,7 @@
       </c>
       <c r="L35" s="93">
         <f t="shared" si="4"/>
-        <v>3917.5214014524076</v>
+        <v>3966.5846914004251</v>
       </c>
       <c r="M35" s="109">
         <v>23585.274397912446</v>
@@ -22750,11 +22750,11 @@
       </c>
       <c r="F36" s="93">
         <f t="shared" si="0"/>
-        <v>1.5356899038496987</v>
+        <v>1.5549958867163853</v>
       </c>
       <c r="G36" s="93">
         <f t="shared" si="1"/>
-        <v>3903.8687368907258</v>
+        <v>3952.9463682271512</v>
       </c>
       <c r="H36" s="108">
         <f>'Bates Grain Kn Calculator'!N38-'Bates Grain Kn Calculator'!N39</f>
@@ -22773,7 +22773,7 @@
       </c>
       <c r="L36" s="93">
         <f t="shared" si="4"/>
-        <v>3903.8687368907258</v>
+        <v>3952.9463682271512</v>
       </c>
       <c r="M36" s="109">
         <v>24738.473231967266</v>
@@ -22803,11 +22803,11 @@
       </c>
       <c r="F37" s="93">
         <f t="shared" si="0"/>
-        <v>1.534918003254798</v>
+        <v>1.5543306032071489</v>
       </c>
       <c r="G37" s="93">
         <f t="shared" si="1"/>
-        <v>3882.2818819919044</v>
+        <v>3931.3823452854199</v>
       </c>
       <c r="H37" s="108">
         <f>'Bates Grain Kn Calculator'!N39-'Bates Grain Kn Calculator'!N40</f>
@@ -22826,7 +22826,7 @@
       </c>
       <c r="L37" s="93">
         <f t="shared" si="4"/>
-        <v>3882.2818819919044</v>
+        <v>3931.3823452854199</v>
       </c>
       <c r="M37" s="109">
         <v>25887.842780290346</v>
@@ -22856,11 +22856,11 @@
       </c>
       <c r="F38" s="93">
         <f t="shared" si="0"/>
-        <v>1.5338572069832028</v>
+        <v>1.5534168966344635</v>
       </c>
       <c r="G38" s="93">
         <f t="shared" si="1"/>
-        <v>3852.886636775851</v>
+        <v>3902.0185028542105</v>
       </c>
       <c r="H38" s="108">
         <f>'Bates Grain Kn Calculator'!N40-'Bates Grain Kn Calculator'!N41</f>
@@ -22879,7 +22879,7 @@
       </c>
       <c r="L38" s="93">
         <f t="shared" si="4"/>
-        <v>3852.886636775851</v>
+        <v>3902.0185028542105</v>
       </c>
       <c r="M38" s="109">
         <v>27031.98307524819</v>
@@ -22909,11 +22909,11 @@
       </c>
       <c r="F39" s="93">
         <f t="shared" si="0"/>
-        <v>1.5325045874701184</v>
+        <v>1.5522527874706873</v>
       </c>
       <c r="G39" s="93">
         <f t="shared" si="1"/>
-        <v>3815.8536039584455</v>
+        <v>3865.02555473757</v>
       </c>
       <c r="H39" s="108">
         <f>'Bates Grain Kn Calculator'!N41-'Bates Grain Kn Calculator'!N42</f>
@@ -22932,7 +22932,7 @@
       </c>
       <c r="L39" s="93">
         <f t="shared" si="4"/>
-        <v>3815.8536039584455</v>
+        <v>3865.02555473757</v>
       </c>
       <c r="M39" s="109">
         <v>28169.510768493841</v>
@@ -22962,11 +22962,11 @@
       </c>
       <c r="F40" s="93">
         <f t="shared" si="0"/>
-        <v>1.5308563851369961</v>
+        <v>1.5508357395555059</v>
       </c>
       <c r="G40" s="93">
         <f t="shared" si="1"/>
-        <v>3771.3965535388102</v>
+        <v>3820.6174139196191</v>
       </c>
       <c r="H40" s="108">
         <f>'Bates Grain Kn Calculator'!N42-'Bates Grain Kn Calculator'!N43</f>
@@ -22985,7 +22985,7 @@
       </c>
       <c r="L40" s="93">
         <f t="shared" si="4"/>
-        <v>3771.3965535388102</v>
+        <v>3820.6174139196191</v>
       </c>
       <c r="M40" s="109">
         <v>29299.063454425461</v>
@@ -23015,11 +23015,11 @@
       </c>
       <c r="F41" s="93">
         <f t="shared" si="0"/>
-        <v>1.5289079782662429</v>
+        <v>1.5491626441715651</v>
       </c>
       <c r="G41" s="93">
         <f t="shared" si="1"/>
-        <v>3719.7703843769095</v>
+        <v>3769.0491555332374</v>
       </c>
       <c r="H41" s="108">
         <f>'Bates Grain Kn Calculator'!N43-'Bates Grain Kn Calculator'!N44</f>
@@ -23038,7 +23038,7 @@
       </c>
       <c r="L41" s="93">
         <f t="shared" si="4"/>
-        <v>3719.7703843769095</v>
+        <v>3769.0491555332374</v>
       </c>
       <c r="M41" s="109">
         <v>30419.3038758195</v>
@@ -23068,11 +23068,11 @@
       </c>
       <c r="F42" s="93">
         <f t="shared" si="0"/>
-        <v>1.5266538455050014</v>
+        <v>1.5472298002988243</v>
       </c>
       <c r="G42" s="93">
         <f t="shared" si="1"/>
-        <v>3661.2687096002337</v>
+        <v>3710.6146040075237</v>
       </c>
       <c r="H42" s="108">
         <f>'Bates Grain Kn Calculator'!N44-'Bates Grain Kn Calculator'!N45</f>
@@ -23091,7 +23091,7 @@
       </c>
       <c r="L42" s="93">
         <f t="shared" si="4"/>
-        <v>3661.2687096002337</v>
+        <v>3710.6146040075237</v>
       </c>
       <c r="M42" s="109">
         <v>31528.923988280818</v>
@@ -23123,11 +23123,11 @@
       </c>
       <c r="F43" s="97">
         <f t="shared" si="0"/>
-        <v>1.5240875204056743</v>
+        <v>1.5450328907828665</v>
       </c>
       <c r="G43" s="97">
         <f t="shared" si="1"/>
-        <v>3596.2210974122804</v>
+        <v>3645.6435760003365</v>
       </c>
       <c r="H43" s="112">
         <f>H42</f>
@@ -23146,7 +23146,7 @@
       </c>
       <c r="L43" s="97">
         <f t="shared" si="4"/>
-        <v>3596.2210974122804</v>
+        <v>3645.6435760003365</v>
       </c>
       <c r="M43" s="113">
         <v>32626.648861105939</v>
@@ -31465,6 +31465,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J9:K9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F2:G2"/>
@@ -31479,15 +31488,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J9:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>